<commit_message>
nginx pm2 tar node
</commit_message>
<xml_diff>
--- a/project_doc/baima/bm消息路由.xlsx
+++ b/project_doc/baima/bm消息路由.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="116">
   <si>
     <t>水资源管理</t>
   </si>
@@ -329,23 +329,6 @@
   </si>
   <si>
     <t>/practice-audit-leader</t>
-  </si>
-  <si>
-    <r>
-      <t>/practice-audit-bm</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>?id=16000-3</t>
-    </r>
-    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>/practice-audit-bm?id=16000-6</t>
@@ -407,6 +390,119 @@
   </si>
   <si>
     <t>/edures-staff</t>
+  </si>
+  <si>
+    <r>
+      <t>/practice-audit-bm</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>?id=16000-3</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>/practice-audit-bm</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>/practice-audit-hq</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>申请人：/practice
+基地：/practice-audit-bm?id=16000-3</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>申请人：/practice
+基地：/practice-audit-bm</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>基地管理员："/repair?id=16000-3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>"
+后勤管理员："/repair</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>?id=16000-6</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>"</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>基地管理员："/repair</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-bm</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+后勤管理员："/repair</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-hq</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>移动端改</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -462,7 +558,7 @@
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -478,6 +574,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFDCE6F1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -570,7 +672,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -608,29 +710,39 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1001,10 +1113,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F50"/>
+  <dimension ref="A1:H50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="F50" sqref="F50"/>
+    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
+      <selection activeCell="B14" sqref="A14:XFD14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1014,10 +1126,11 @@
     <col min="3" max="3" width="21.75" customWidth="1"/>
     <col min="4" max="4" width="71.875" customWidth="1"/>
     <col min="5" max="5" width="37.375" customWidth="1"/>
-    <col min="6" max="6" width="29.875" style="15" customWidth="1"/>
+    <col min="6" max="6" width="40.375" style="13" customWidth="1"/>
+    <col min="8" max="8" width="28" style="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1026,7 +1139,7 @@
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
     </row>
-    <row r="2" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -1045,8 +1158,11 @@
       <c r="F2" s="3" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="42.75" x14ac:dyDescent="0.15">
+      <c r="H2" s="22" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
@@ -1062,11 +1178,11 @@
       <c r="E3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="15" t="s">
+      <c r="F3" s="13" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="42.75" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A4" s="4" t="s">
         <v>11</v>
       </c>
@@ -1080,11 +1196,11 @@
         <v>9</v>
       </c>
       <c r="E4" s="4"/>
-      <c r="F4" s="15" t="s">
+      <c r="F4" s="13" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="46.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:8" ht="46.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="4" t="s">
         <v>14</v>
       </c>
@@ -1100,11 +1216,11 @@
       <c r="E5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="15" t="s">
+      <c r="F5" s="13" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="42.75" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:8" ht="28.5" x14ac:dyDescent="0.15">
       <c r="A6" s="4" t="s">
         <v>19</v>
       </c>
@@ -1124,7 +1240,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="62.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:8" ht="62.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="4" t="s">
         <v>23</v>
       </c>
@@ -1137,14 +1253,14 @@
       <c r="D7" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="16" t="s">
+      <c r="E7" s="14" t="s">
         <v>97</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A8" s="4" t="s">
         <v>26</v>
       </c>
@@ -1155,7 +1271,7 @@
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
     </row>
-    <row r="11" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
         <v>28</v>
       </c>
@@ -1164,7 +1280,7 @@
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
     </row>
-    <row r="12" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A12" s="3" t="s">
         <v>1</v>
       </c>
@@ -1180,11 +1296,11 @@
       <c r="E12" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F12" s="15" t="s">
+      <c r="F12" s="13" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="42.75" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A13" s="4" t="s">
         <v>29</v>
       </c>
@@ -1200,11 +1316,11 @@
       <c r="E13" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="F13" s="15" t="s">
+      <c r="F13" s="13" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="42.75" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A14" s="4" t="s">
         <v>33</v>
       </c>
@@ -1217,14 +1333,17 @@
       <c r="D14" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E14" s="16" t="s">
+      <c r="E14" s="14" t="s">
         <v>98</v>
       </c>
-      <c r="F14" s="18" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="28.5" x14ac:dyDescent="0.15">
+      <c r="F14" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="H14" s="23" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="28.5" x14ac:dyDescent="0.15">
       <c r="A15" s="4" t="s">
         <v>34</v>
       </c>
@@ -1240,11 +1359,11 @@
       <c r="E15" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="F15" s="15" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="42.75" x14ac:dyDescent="0.15">
+      <c r="F15" s="13" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A16" s="4" t="s">
         <v>37</v>
       </c>
@@ -1260,11 +1379,14 @@
       <c r="E16" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="F16" s="18" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="28.5" x14ac:dyDescent="0.15">
+      <c r="F16" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="H16" s="23" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="28.5" x14ac:dyDescent="0.15">
       <c r="A17" s="4" t="s">
         <v>41</v>
       </c>
@@ -1280,11 +1402,11 @@
       <c r="E17" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="F17" s="15" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="40.5" x14ac:dyDescent="0.15">
+      <c r="F17" s="13" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A18" s="4" t="s">
         <v>42</v>
       </c>
@@ -1300,11 +1422,14 @@
       <c r="E18" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="F18" s="17" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="40.5" x14ac:dyDescent="0.15">
+      <c r="F18" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="H18" s="24" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A19" s="4" t="s">
         <v>45</v>
       </c>
@@ -1320,11 +1445,14 @@
       <c r="E19" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="F19" s="17" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="F19" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="H19" s="24" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A20" s="4" t="s">
         <v>47</v>
       </c>
@@ -1335,7 +1463,7 @@
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
     </row>
-    <row r="24" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A24" s="1" t="s">
         <v>49</v>
       </c>
@@ -1344,7 +1472,7 @@
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="1:6" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A25" s="3" t="s">
         <v>1</v>
       </c>
@@ -1360,11 +1488,11 @@
       <c r="E25" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F25" s="15" t="s">
+      <c r="F25" s="13" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="57" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:8" ht="57" x14ac:dyDescent="0.15">
       <c r="A26" s="4" t="s">
         <v>50</v>
       </c>
@@ -1380,11 +1508,14 @@
       <c r="E26" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="F26" s="16" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="57" x14ac:dyDescent="0.15">
+      <c r="F26" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="H26" s="22" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="57" x14ac:dyDescent="0.15">
       <c r="A27" s="4" t="s">
         <v>54</v>
       </c>
@@ -1400,11 +1531,14 @@
       <c r="E27" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="F27" s="16" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="42.75" x14ac:dyDescent="0.15">
+      <c r="F27" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="H27" s="22" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A28" s="4" t="s">
         <v>55</v>
       </c>
@@ -1420,11 +1554,11 @@
       <c r="E28" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="F28" s="15" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="57" x14ac:dyDescent="0.15">
+      <c r="F28" s="13" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="57" x14ac:dyDescent="0.15">
       <c r="A29" s="4" t="s">
         <v>60</v>
       </c>
@@ -1440,11 +1574,14 @@
       <c r="E29" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="F29" s="16" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="57" x14ac:dyDescent="0.15">
+      <c r="F29" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="H29" s="22" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="57" x14ac:dyDescent="0.15">
       <c r="A30" s="4" t="s">
         <v>63</v>
       </c>
@@ -1460,11 +1597,14 @@
       <c r="E30" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="F30" s="16" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="14.25" thickBot="1" x14ac:dyDescent="0.2"/>
+      <c r="F30" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="H30" s="22" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="14.25" thickBot="1" x14ac:dyDescent="0.2"/>
     <row r="33" spans="1:6" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A33" s="5" t="s">
         <v>66</v>
@@ -1491,7 +1631,7 @@
       <c r="E34" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="F34" s="19" t="s">
+      <c r="F34" s="17" t="s">
         <v>91</v>
       </c>
     </row>
@@ -1511,8 +1651,8 @@
       <c r="E35" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="F35" s="20" t="s">
-        <v>106</v>
+      <c r="F35" s="18" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="41.25" thickBot="1" x14ac:dyDescent="0.2">
@@ -1531,8 +1671,8 @@
       <c r="E36" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="F36" s="20" t="s">
-        <v>107</v>
+      <c r="F36" s="18" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
@@ -1552,7 +1692,7 @@
         <v>72</v>
       </c>
       <c r="F37" s="11" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="27.75" thickBot="1" x14ac:dyDescent="0.2">
@@ -1572,7 +1712,7 @@
         <v>72</v>
       </c>
       <c r="F38" s="11" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
@@ -1592,7 +1732,7 @@
         <v>72</v>
       </c>
       <c r="F39" s="11" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="41.25" thickBot="1" x14ac:dyDescent="0.2">
@@ -1611,8 +1751,8 @@
       <c r="E40" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="F40" s="20" t="s">
-        <v>107</v>
+      <c r="F40" s="18" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="27.75" thickBot="1" x14ac:dyDescent="0.2">
@@ -1632,7 +1772,7 @@
         <v>72</v>
       </c>
       <c r="F41" s="11" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
@@ -1652,7 +1792,7 @@
         <v>72</v>
       </c>
       <c r="F42" s="11" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="41.25" thickBot="1" x14ac:dyDescent="0.2">
@@ -1671,8 +1811,8 @@
       <c r="E43" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="F43" s="20" t="s">
-        <v>107</v>
+      <c r="F43" s="18" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
@@ -1692,7 +1832,7 @@
         <v>72</v>
       </c>
       <c r="F44" s="11" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
@@ -1712,7 +1852,7 @@
         <v>72</v>
       </c>
       <c r="F45" s="11" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
@@ -1732,7 +1872,7 @@
         <v>72</v>
       </c>
       <c r="F46" s="11" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="27.75" thickBot="1" x14ac:dyDescent="0.2">
@@ -1752,7 +1892,7 @@
         <v>85</v>
       </c>
       <c r="F47" s="10" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
@@ -1772,7 +1912,7 @@
         <v>85</v>
       </c>
       <c r="F48" s="11" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
@@ -1784,17 +1924,17 @@
       <c r="F49" s="11"/>
     </row>
     <row r="50" spans="1:6" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="13" t="s">
+      <c r="A50" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="B50" s="14"/>
-      <c r="C50" s="14"/>
-      <c r="D50" s="14"/>
+      <c r="B50" s="20"/>
+      <c r="C50" s="20"/>
+      <c r="D50" s="20"/>
       <c r="E50" s="11" t="s">
         <v>72</v>
       </c>
       <c r="F50" s="10" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>

</xml_diff>